<commit_message>
sprint review document filled out
</commit_message>
<xml_diff>
--- a/TutorGroup_SprintBacklog.xlsx
+++ b/TutorGroup_SprintBacklog.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahyelle/Desktop/Tutor-Software-Engineering/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957F9706-2750-3A4A-AE16-3F805666EC56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjR5WleU3OGRlUjTv6BiiKH/UrtfA=="/>
@@ -16,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Number</t>
   </si>
@@ -50,39 +59,46 @@
   <si>
     <t>As a general user I would like the main features to be accessible from the home page, as I will be using the main features the most.</t>
   </si>
+  <si>
+    <t>Hannah -- 100%, still need to fix errors and do backend</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7">
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="&quot;Times New Roman&quot;"/>
     </font>
     <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
     </font>
@@ -92,53 +108,58 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -328,28 +349,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.56"/>
-    <col customWidth="1" min="2" max="2" width="98.33"/>
-    <col customWidth="1" min="3" max="4" width="10.56"/>
-    <col customWidth="1" min="5" max="5" width="19.11"/>
-    <col customWidth="1" min="6" max="6" width="30.44"/>
-    <col customWidth="1" min="7" max="26" width="10.56"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="98.28515625" customWidth="1"/>
+    <col min="3" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1"/>
+    <col min="7" max="26" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="42.75" customHeight="1">
+    <row r="1" spans="1:26" ht="42.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -389,9 +412,9 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" ht="27.0" customHeight="1">
+    <row r="2" spans="1:26" ht="27" customHeight="1">
       <c r="A2" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>6</v>
@@ -400,15 +423,18 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E2" s="5">
-        <v>0.0</v>
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" ht="28.5" customHeight="1">
+    <row r="3" spans="1:26" ht="28.5" customHeight="1">
       <c r="A3" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -417,15 +443,15 @@
         <v>7</v>
       </c>
       <c r="D3" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E3" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="4" ht="22.5" customHeight="1">
+    <row r="4" spans="1:26" ht="22.5" customHeight="1">
       <c r="A4" s="3">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>9</v>
@@ -434,15 +460,15 @@
         <v>7</v>
       </c>
       <c r="D4" s="6">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E4" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="5" ht="24.75" customHeight="1">
+    <row r="5" spans="1:26" ht="24.75" customHeight="1">
       <c r="A5" s="3">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>10</v>
@@ -451,29 +477,29 @@
         <v>7</v>
       </c>
       <c r="D5" s="6">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E5" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:26" ht="15.75" customHeight="1">
       <c r="B6" s="8"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:26" ht="15.75" customHeight="1">
       <c r="B7" s="8"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:26" ht="15.75" customHeight="1">
       <c r="B8" s="8"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -1459,9 +1485,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>